<commit_message>
UPDATED EXCEL ASSIGNMENT SHEET
</commit_message>
<xml_diff>
--- a/assignment 1.xlsx
+++ b/assignment 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\i0261959\Desktop\Soliqua\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1007CD6-94FD-481B-B192-294BE8070955}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD5B27E-F921-4D27-927A-1A4776D00F2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{4DF7B232-5003-482D-8C8F-21A13FE7C0FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4DF7B232-5003-482D-8C8F-21A13FE7C0FF}"/>
   </bookViews>
   <sheets>
     <sheet name="flashfill" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="138">
   <si>
     <t>First Name</t>
   </si>
@@ -402,30 +402,6 @@
   </si>
   <si>
     <t>COUNT OF ALL THE EMPLOYEE</t>
-  </si>
-  <si>
-    <t>B100</t>
-  </si>
-  <si>
-    <t>C101</t>
-  </si>
-  <si>
-    <t>M102</t>
-  </si>
-  <si>
-    <t>Q103</t>
-  </si>
-  <si>
-    <t>S104</t>
-  </si>
-  <si>
-    <t>R234</t>
-  </si>
-  <si>
-    <t>H898</t>
-  </si>
-  <si>
-    <t>J345</t>
   </si>
   <si>
     <t>SHRADDHA MULE</t>
@@ -934,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED2A47A0-F2C7-4CD1-8432-551D5C9EDCC0}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,8 +958,8 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>121</v>
+      <c r="F2" s="1">
+        <v>100</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
@@ -1002,8 +978,8 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>122</v>
+      <c r="F3" s="1">
+        <v>101</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>12</v>
@@ -1022,8 +998,8 @@
       <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>123</v>
+      <c r="F4" s="1">
+        <v>102</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>13</v>
@@ -1042,8 +1018,8 @@
       <c r="E5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>124</v>
+      <c r="F5" s="1">
+        <v>103</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>14</v>
@@ -1062,8 +1038,8 @@
       <c r="E6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>125</v>
+      <c r="F6" s="1">
+        <v>104</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>15</v>
@@ -1082,8 +1058,8 @@
       <c r="E7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>126</v>
+      <c r="F7" s="1">
+        <v>234</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>16</v>
@@ -1102,8 +1078,8 @@
       <c r="E8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>127</v>
+      <c r="F8" s="1">
+        <v>898</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>17</v>
@@ -1122,8 +1098,8 @@
       <c r="E9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>128</v>
+      <c r="F9" s="1">
+        <v>345</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>18</v>
@@ -1157,7 +1133,7 @@
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>24</v>
@@ -1166,10 +1142,10 @@
         <v>25</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1177,7 +1153,7 @@
         <v>26</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>27</v>
@@ -1186,10 +1162,10 @@
         <v>6</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1197,7 +1173,7 @@
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>29</v>
@@ -1206,10 +1182,10 @@
         <v>30</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1217,7 +1193,7 @@
         <v>31</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>32</v>
@@ -1226,10 +1202,10 @@
         <v>33</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1237,7 +1213,7 @@
         <v>34</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>35</v>
@@ -1246,10 +1222,10 @@
         <v>4</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1257,7 +1233,7 @@
         <v>36</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>37</v>
@@ -1266,10 +1242,10 @@
         <v>5</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1277,7 +1253,7 @@
         <v>38</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -1912,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14E4265-5E4D-4AAE-A711-5F389043BFC9}">
   <dimension ref="A1:F247"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>